<commit_message>
Sort array of 0s 1s and 2s
</commit_message>
<xml_diff>
--- a/crashSheetDSA.xlsx
+++ b/crashSheetDSA.xlsx
@@ -49,10 +49,10 @@
     <t xml:space="preserve">Find the "Kth" max and min element of an array </t>
   </si>
   <si>
+    <t xml:space="preserve">Given an array which consists of only 0, 1 and 2. Sort the array without using any sorting algo</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;-&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given an array which consists of only 0, 1 and 2. Sort the array without using any sorting algo</t>
   </si>
   <si>
     <t xml:space="preserve">Move all the negative elements to one side of the array </t>
@@ -1659,10 +1659,10 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -1688,7 +1688,7 @@
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,10 +1726,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,7 +1740,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1751,7 +1751,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,7 +1762,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,7 +1773,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,7 +1784,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,7 +1795,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,7 +1806,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1817,7 +1817,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,7 +1828,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,7 +1839,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,7 +1850,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,7 +1861,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,7 +1872,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,7 +1883,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +1894,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,7 +1905,7 @@
         <v>26</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,7 +1916,7 @@
         <v>27</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,7 +1927,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,7 +1938,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,7 +1949,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1960,7 +1960,7 @@
         <v>31</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,7 +1971,7 @@
         <v>32</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,7 +1982,7 @@
         <v>33</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1993,7 +1993,7 @@
         <v>34</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,7 +2004,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,7 +2015,7 @@
         <v>36</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,7 +2026,7 @@
         <v>37</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2037,7 +2037,7 @@
         <v>38</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2048,7 +2048,7 @@
         <v>39</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,7 +2059,7 @@
         <v>40</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,7 +2070,7 @@
         <v>41</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2081,20 +2081,20 @@
         <v>42</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="7"/>
       <c r="C42" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
       <c r="C43" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,7 +2105,7 @@
         <v>44</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,7 +2116,7 @@
         <v>45</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2127,7 +2127,7 @@
         <v>46</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,7 +2138,7 @@
         <v>47</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,7 +2149,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,7 +2160,7 @@
         <v>49</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,7 +2171,7 @@
         <v>50</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2182,7 +2182,7 @@
         <v>51</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,7 +2193,7 @@
         <v>52</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,7 +2204,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,7 +2220,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,7 +2231,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,7 +2242,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,7 +2253,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,7 +2264,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2275,7 +2275,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,7 +2286,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,7 +2297,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,7 +2308,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,7 +2319,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,7 +2330,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,7 +2341,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2352,7 +2352,7 @@
         <v>67</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,7 +2363,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2374,7 +2374,7 @@
         <v>69</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,7 +2385,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,7 +2396,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,7 +2407,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,7 +2418,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2429,7 +2429,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2440,7 +2440,7 @@
         <v>75</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,7 +2451,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,7 +2462,7 @@
         <v>77</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,7 +2473,7 @@
         <v>78</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,7 +2484,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,7 +2495,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,7 +2506,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2517,7 +2517,7 @@
         <v>82</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,7 +2528,7 @@
         <v>83</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,7 +2539,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,7 +2550,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2561,7 +2561,7 @@
         <v>86</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,7 +2572,7 @@
         <v>87</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,7 +2583,7 @@
         <v>88</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,7 +2594,7 @@
         <v>89</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,7 +2605,7 @@
         <v>90</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2616,7 @@
         <v>91</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,7 +2627,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,7 +2638,7 @@
         <v>93</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2649,7 +2649,7 @@
         <v>94</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,7 +2660,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2671,7 +2671,7 @@
         <v>96</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,7 +2682,7 @@
         <v>97</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2698,7 +2698,7 @@
         <v>99</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,7 +2709,7 @@
         <v>100</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2720,7 +2720,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2731,7 +2731,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +2742,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,7 +2753,7 @@
         <v>104</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2764,7 +2764,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2775,7 +2775,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2786,7 +2786,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,7 +2797,7 @@
         <v>108</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2808,7 +2808,7 @@
         <v>109</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2819,7 +2819,7 @@
         <v>110</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,7 +2830,7 @@
         <v>111</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2841,7 +2841,7 @@
         <v>112</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2852,7 +2852,7 @@
         <v>113</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2863,7 +2863,7 @@
         <v>114</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2874,7 +2874,7 @@
         <v>115</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2885,7 +2885,7 @@
         <v>116</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2896,7 +2896,7 @@
         <v>117</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2907,7 +2907,7 @@
         <v>118</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2918,7 +2918,7 @@
         <v>119</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2929,7 +2929,7 @@
         <v>120</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2940,7 +2940,7 @@
         <v>121</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2951,7 +2951,7 @@
         <v>122</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,7 +2962,7 @@
         <v>123</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2973,7 +2973,7 @@
         <v>124</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2984,7 +2984,7 @@
         <v>125</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,7 +2995,7 @@
         <v>126</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3006,7 +3006,7 @@
         <v>127</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3017,7 +3017,7 @@
         <v>128</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,7 +3028,7 @@
         <v>129</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3039,7 +3039,7 @@
         <v>130</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3050,7 +3050,7 @@
         <v>131</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3061,7 +3061,7 @@
         <v>132</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3072,7 +3072,7 @@
         <v>133</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,7 +3083,7 @@
         <v>134</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3098,7 +3098,7 @@
         <v>136</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3109,7 +3109,7 @@
         <v>137</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3120,7 +3120,7 @@
         <v>138</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,7 +3131,7 @@
         <v>139</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3142,7 +3142,7 @@
         <v>140</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3153,7 +3153,7 @@
         <v>141</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,7 +3164,7 @@
         <v>142</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3175,7 +3175,7 @@
         <v>143</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,7 +3186,7 @@
         <v>144</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,7 +3197,7 @@
         <v>145</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3208,7 +3208,7 @@
         <v>146</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3219,7 +3219,7 @@
         <v>147</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3230,7 +3230,7 @@
         <v>148</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3241,7 +3241,7 @@
         <v>149</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,7 +3252,7 @@
         <v>150</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,7 +3263,7 @@
         <v>151</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,7 +3274,7 @@
         <v>152</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,7 +3285,7 @@
         <v>153</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,7 +3296,7 @@
         <v>154</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,7 +3307,7 @@
         <v>155</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3318,7 +3318,7 @@
         <v>156</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,7 +3329,7 @@
         <v>157</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3340,7 +3340,7 @@
         <v>158</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3351,7 +3351,7 @@
         <v>159</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3362,7 +3362,7 @@
         <v>160</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3373,7 +3373,7 @@
         <v>161</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3384,7 +3384,7 @@
         <v>162</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3395,7 +3395,7 @@
         <v>163</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3406,7 +3406,7 @@
         <v>164</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3417,7 +3417,7 @@
         <v>165</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3428,7 +3428,7 @@
         <v>166</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3439,7 +3439,7 @@
         <v>167</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3450,7 +3450,7 @@
         <v>168</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3461,7 +3461,7 @@
         <v>169</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,7 +3472,7 @@
         <v>170</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3483,7 +3483,7 @@
         <v>171</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3498,7 +3498,7 @@
         <v>173</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3509,7 +3509,7 @@
         <v>174</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3520,7 +3520,7 @@
         <v>175</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3531,7 +3531,7 @@
         <v>176</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3542,7 +3542,7 @@
         <v>177</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3553,7 +3553,7 @@
         <v>178</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3564,7 +3564,7 @@
         <v>179</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,7 +3575,7 @@
         <v>180</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3586,7 +3586,7 @@
         <v>181</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3597,7 +3597,7 @@
         <v>182</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3608,7 +3608,7 @@
         <v>183</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3619,7 +3619,7 @@
         <v>184</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3630,7 +3630,7 @@
         <v>185</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3641,7 +3641,7 @@
         <v>186</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3652,7 +3652,7 @@
         <v>187</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3663,7 +3663,7 @@
         <v>188</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3674,7 +3674,7 @@
         <v>189</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3685,7 +3685,7 @@
         <v>190</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3696,7 +3696,7 @@
         <v>191</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3707,7 +3707,7 @@
         <v>192</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3718,7 +3718,7 @@
         <v>193</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3729,7 +3729,7 @@
         <v>194</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3740,7 +3740,7 @@
         <v>195</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3751,7 +3751,7 @@
         <v>196</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3762,7 +3762,7 @@
         <v>197</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3773,7 +3773,7 @@
         <v>198</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,7 +3784,7 @@
         <v>199</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3795,7 +3795,7 @@
         <v>200</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3806,7 +3806,7 @@
         <v>201</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3817,7 +3817,7 @@
         <v>202</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3828,7 +3828,7 @@
         <v>203</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3839,7 +3839,7 @@
         <v>204</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3850,7 +3850,7 @@
         <v>205</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3861,7 +3861,7 @@
         <v>206</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3872,7 +3872,7 @@
         <v>207</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3893,7 +3893,7 @@
         <v>209</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3904,7 +3904,7 @@
         <v>210</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3915,7 +3915,7 @@
         <v>211</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3926,7 +3926,7 @@
         <v>212</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3937,7 +3937,7 @@
         <v>213</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3948,7 +3948,7 @@
         <v>214</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3959,7 +3959,7 @@
         <v>215</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3970,7 +3970,7 @@
         <v>216</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3981,7 +3981,7 @@
         <v>217</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3992,7 +3992,7 @@
         <v>218</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,7 +4003,7 @@
         <v>219</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4014,7 +4014,7 @@
         <v>220</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4025,7 +4025,7 @@
         <v>221</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4036,7 +4036,7 @@
         <v>222</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4047,7 +4047,7 @@
         <v>223</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4058,7 +4058,7 @@
         <v>224</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4069,7 +4069,7 @@
         <v>225</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4080,7 +4080,7 @@
         <v>226</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4091,7 +4091,7 @@
         <v>227</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4102,7 +4102,7 @@
         <v>228</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4113,7 +4113,7 @@
         <v>229</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4124,7 +4124,7 @@
         <v>230</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4143,7 +4143,7 @@
         <v>232</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4154,7 +4154,7 @@
         <v>233</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4165,7 +4165,7 @@
         <v>234</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4176,7 +4176,7 @@
         <v>235</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4187,7 +4187,7 @@
         <v>236</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4198,7 +4198,7 @@
         <v>237</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4209,7 +4209,7 @@
         <v>238</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4220,7 +4220,7 @@
         <v>239</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4231,7 +4231,7 @@
         <v>240</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4242,7 +4242,7 @@
         <v>241</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4253,7 +4253,7 @@
         <v>242</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4264,7 +4264,7 @@
         <v>243</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4275,7 +4275,7 @@
         <v>244</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4286,7 +4286,7 @@
         <v>245</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4297,7 +4297,7 @@
         <v>246</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4308,7 +4308,7 @@
         <v>247</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4319,7 +4319,7 @@
         <v>248</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4330,7 +4330,7 @@
         <v>249</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4341,7 +4341,7 @@
         <v>250</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4352,7 +4352,7 @@
         <v>251</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4363,7 +4363,7 @@
         <v>252</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,7 +4374,7 @@
         <v>253</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4385,7 +4385,7 @@
         <v>254</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4396,7 +4396,7 @@
         <v>255</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4407,7 +4407,7 @@
         <v>256</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4418,7 +4418,7 @@
         <v>257</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4429,7 +4429,7 @@
         <v>258</v>
       </c>
       <c r="C264" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4440,7 +4440,7 @@
         <v>259</v>
       </c>
       <c r="C265" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4451,7 +4451,7 @@
         <v>260</v>
       </c>
       <c r="C266" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4462,7 +4462,7 @@
         <v>261</v>
       </c>
       <c r="C267" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4473,7 +4473,7 @@
         <v>262</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4484,7 +4484,7 @@
         <v>263</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4495,7 +4495,7 @@
         <v>264</v>
       </c>
       <c r="C270" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4506,7 +4506,7 @@
         <v>88</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4517,7 +4517,7 @@
         <v>265</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,7 +4536,7 @@
         <v>267</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4547,7 +4547,7 @@
         <v>268</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4558,7 +4558,7 @@
         <v>269</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4569,7 +4569,7 @@
         <v>270</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4580,7 +4580,7 @@
         <v>271</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4591,7 +4591,7 @@
         <v>272</v>
       </c>
       <c r="C280" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4602,7 +4602,7 @@
         <v>273</v>
       </c>
       <c r="C281" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4613,7 +4613,7 @@
         <v>274</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4624,7 +4624,7 @@
         <v>275</v>
       </c>
       <c r="C283" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4635,7 +4635,7 @@
         <v>276</v>
       </c>
       <c r="C284" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4646,7 +4646,7 @@
         <v>277</v>
       </c>
       <c r="C285" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4657,7 +4657,7 @@
         <v>278</v>
       </c>
       <c r="C286" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4668,7 +4668,7 @@
         <v>279</v>
       </c>
       <c r="C287" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4679,7 +4679,7 @@
         <v>280</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4690,7 +4690,7 @@
         <v>281</v>
       </c>
       <c r="C289" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4701,7 +4701,7 @@
         <v>282</v>
       </c>
       <c r="C290" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4712,7 +4712,7 @@
         <v>283</v>
       </c>
       <c r="C291" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4723,7 +4723,7 @@
         <v>284</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4734,7 +4734,7 @@
         <v>285</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4753,7 +4753,7 @@
         <v>287</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4764,7 +4764,7 @@
         <v>288</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4775,7 +4775,7 @@
         <v>289</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4786,7 +4786,7 @@
         <v>290</v>
       </c>
       <c r="C299" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4797,7 +4797,7 @@
         <v>291</v>
       </c>
       <c r="C300" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4808,7 +4808,7 @@
         <v>292</v>
       </c>
       <c r="C301" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4819,7 +4819,7 @@
         <v>293</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4830,7 +4830,7 @@
         <v>294</v>
       </c>
       <c r="C303" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4841,7 +4841,7 @@
         <v>295</v>
       </c>
       <c r="C304" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4852,7 +4852,7 @@
         <v>296</v>
       </c>
       <c r="C305" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4863,7 +4863,7 @@
         <v>297</v>
       </c>
       <c r="C306" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4874,7 +4874,7 @@
         <v>298</v>
       </c>
       <c r="C307" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4885,7 +4885,7 @@
         <v>299</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4896,7 +4896,7 @@
         <v>300</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4907,7 +4907,7 @@
         <v>301</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4918,7 +4918,7 @@
         <v>302</v>
       </c>
       <c r="C311" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4929,7 +4929,7 @@
         <v>303</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4940,7 +4940,7 @@
         <v>304</v>
       </c>
       <c r="C313" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4951,7 +4951,7 @@
         <v>305</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4962,7 +4962,7 @@
         <v>306</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4973,7 +4973,7 @@
         <v>307</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4984,7 +4984,7 @@
         <v>308</v>
       </c>
       <c r="C317" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4995,7 +4995,7 @@
         <v>309</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5006,7 +5006,7 @@
         <v>310</v>
       </c>
       <c r="C319" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5017,7 +5017,7 @@
         <v>311</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5028,7 +5028,7 @@
         <v>312</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5039,7 +5039,7 @@
         <v>313</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5050,7 +5050,7 @@
         <v>314</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5061,7 +5061,7 @@
         <v>315</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5072,7 +5072,7 @@
         <v>316</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5083,7 +5083,7 @@
         <v>317</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5094,7 +5094,7 @@
         <v>318</v>
       </c>
       <c r="C327" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5105,7 +5105,7 @@
         <v>319</v>
       </c>
       <c r="C328" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5116,7 +5116,7 @@
         <v>320</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5127,7 +5127,7 @@
         <v>321</v>
       </c>
       <c r="C330" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5138,7 +5138,7 @@
         <v>322</v>
       </c>
       <c r="C331" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5149,7 +5149,7 @@
         <v>323</v>
       </c>
       <c r="C332" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5160,7 +5160,7 @@
         <v>324</v>
       </c>
       <c r="C333" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5179,7 +5179,7 @@
         <v>326</v>
       </c>
       <c r="C336" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5190,7 +5190,7 @@
         <v>327</v>
       </c>
       <c r="C337" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5201,7 +5201,7 @@
         <v>328</v>
       </c>
       <c r="C338" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5212,7 +5212,7 @@
         <v>329</v>
       </c>
       <c r="C339" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5223,7 +5223,7 @@
         <v>330</v>
       </c>
       <c r="C340" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5234,7 +5234,7 @@
         <v>331</v>
       </c>
       <c r="C341" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5245,7 +5245,7 @@
         <v>332</v>
       </c>
       <c r="C342" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5256,7 +5256,7 @@
         <v>333</v>
       </c>
       <c r="C343" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,7 +5267,7 @@
         <v>334</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5278,7 +5278,7 @@
         <v>335</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5289,7 +5289,7 @@
         <v>336</v>
       </c>
       <c r="C346" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5300,7 +5300,7 @@
         <v>337</v>
       </c>
       <c r="C347" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5311,7 +5311,7 @@
         <v>338</v>
       </c>
       <c r="C348" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5322,7 +5322,7 @@
         <v>339</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5333,7 +5333,7 @@
         <v>340</v>
       </c>
       <c r="C350" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5344,7 +5344,7 @@
         <v>341</v>
       </c>
       <c r="C351" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5355,7 +5355,7 @@
         <v>342</v>
       </c>
       <c r="C352" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5366,7 +5366,7 @@
         <v>343</v>
       </c>
       <c r="C353" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5385,7 +5385,7 @@
         <v>345</v>
       </c>
       <c r="C356" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5396,7 +5396,7 @@
         <v>346</v>
       </c>
       <c r="C357" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5407,7 +5407,7 @@
         <v>347</v>
       </c>
       <c r="C358" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5418,7 +5418,7 @@
         <v>348</v>
       </c>
       <c r="C359" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5429,7 +5429,7 @@
         <v>349</v>
       </c>
       <c r="C360" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5440,7 +5440,7 @@
         <v>350</v>
       </c>
       <c r="C361" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5451,7 +5451,7 @@
         <v>351</v>
       </c>
       <c r="C362" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5462,7 +5462,7 @@
         <v>352</v>
       </c>
       <c r="C363" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5473,7 +5473,7 @@
         <v>353</v>
       </c>
       <c r="C364" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5484,7 +5484,7 @@
         <v>354</v>
       </c>
       <c r="C365" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5495,7 +5495,7 @@
         <v>355</v>
       </c>
       <c r="C366" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5506,7 +5506,7 @@
         <v>356</v>
       </c>
       <c r="C367" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5517,7 +5517,7 @@
         <v>357</v>
       </c>
       <c r="C368" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5528,7 +5528,7 @@
         <v>358</v>
       </c>
       <c r="C369" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5539,7 +5539,7 @@
         <v>359</v>
       </c>
       <c r="C370" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5550,7 +5550,7 @@
         <v>360</v>
       </c>
       <c r="C371" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5561,7 +5561,7 @@
         <v>361</v>
       </c>
       <c r="C372" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5572,7 +5572,7 @@
         <v>362</v>
       </c>
       <c r="C373" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5583,7 +5583,7 @@
         <v>363</v>
       </c>
       <c r="C374" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5594,7 +5594,7 @@
         <v>364</v>
       </c>
       <c r="C375" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5605,7 +5605,7 @@
         <v>365</v>
       </c>
       <c r="C376" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5616,7 +5616,7 @@
         <v>366</v>
       </c>
       <c r="C377" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5627,7 +5627,7 @@
         <v>367</v>
       </c>
       <c r="C378" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5638,7 +5638,7 @@
         <v>368</v>
       </c>
       <c r="C379" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5649,7 +5649,7 @@
         <v>369</v>
       </c>
       <c r="C380" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5660,7 +5660,7 @@
         <v>370</v>
       </c>
       <c r="C381" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5671,7 +5671,7 @@
         <v>371</v>
       </c>
       <c r="C382" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5682,7 +5682,7 @@
         <v>372</v>
       </c>
       <c r="C383" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5693,7 +5693,7 @@
         <v>373</v>
       </c>
       <c r="C384" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5704,7 +5704,7 @@
         <v>374</v>
       </c>
       <c r="C385" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5715,7 +5715,7 @@
         <v>375</v>
       </c>
       <c r="C386" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5726,7 +5726,7 @@
         <v>376</v>
       </c>
       <c r="C387" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5737,7 +5737,7 @@
         <v>377</v>
       </c>
       <c r="C388" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5748,7 +5748,7 @@
         <v>378</v>
       </c>
       <c r="C389" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5759,7 +5759,7 @@
         <v>378</v>
       </c>
       <c r="C390" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5770,7 +5770,7 @@
         <v>379</v>
       </c>
       <c r="C391" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5781,7 +5781,7 @@
         <v>380</v>
       </c>
       <c r="C392" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5792,7 +5792,7 @@
         <v>381</v>
       </c>
       <c r="C393" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5803,7 +5803,7 @@
         <v>382</v>
       </c>
       <c r="C394" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,7 +5814,7 @@
         <v>383</v>
       </c>
       <c r="C395" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5825,7 +5825,7 @@
         <v>384</v>
       </c>
       <c r="C396" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5836,7 +5836,7 @@
         <v>385</v>
       </c>
       <c r="C397" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5847,7 +5847,7 @@
         <v>386</v>
       </c>
       <c r="C398" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5858,7 +5858,7 @@
         <v>387</v>
       </c>
       <c r="C399" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5877,7 +5877,7 @@
         <v>389</v>
       </c>
       <c r="C402" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5888,7 +5888,7 @@
         <v>390</v>
       </c>
       <c r="C403" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5899,7 +5899,7 @@
         <v>391</v>
       </c>
       <c r="C404" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5910,7 +5910,7 @@
         <v>90</v>
       </c>
       <c r="C405" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5921,7 +5921,7 @@
         <v>392</v>
       </c>
       <c r="C406" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5932,7 +5932,7 @@
         <v>393</v>
       </c>
       <c r="C407" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5951,7 +5951,7 @@
         <v>395</v>
       </c>
       <c r="C410" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5962,7 +5962,7 @@
         <v>396</v>
       </c>
       <c r="C411" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5973,7 +5973,7 @@
         <v>397</v>
       </c>
       <c r="C412" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5984,7 +5984,7 @@
         <v>398</v>
       </c>
       <c r="C413" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5995,7 +5995,7 @@
         <v>399</v>
       </c>
       <c r="C414" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6006,7 +6006,7 @@
         <v>400</v>
       </c>
       <c r="C415" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6017,7 +6017,7 @@
         <v>401</v>
       </c>
       <c r="C416" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6028,7 +6028,7 @@
         <v>274</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6039,7 +6039,7 @@
         <v>402</v>
       </c>
       <c r="C418" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6050,7 +6050,7 @@
         <v>403</v>
       </c>
       <c r="C419" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6061,7 +6061,7 @@
         <v>404</v>
       </c>
       <c r="C420" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6072,7 +6072,7 @@
         <v>405</v>
       </c>
       <c r="C421" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6083,7 +6083,7 @@
         <v>406</v>
       </c>
       <c r="C422" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6094,7 +6094,7 @@
         <v>407</v>
       </c>
       <c r="C423" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6105,7 +6105,7 @@
         <v>408</v>
       </c>
       <c r="C424" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6116,7 +6116,7 @@
         <v>409</v>
       </c>
       <c r="C425" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6127,7 +6127,7 @@
         <v>410</v>
       </c>
       <c r="C426" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6138,7 +6138,7 @@
         <v>411</v>
       </c>
       <c r="C427" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6149,7 +6149,7 @@
         <v>412</v>
       </c>
       <c r="C428" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6160,7 +6160,7 @@
         <v>413</v>
       </c>
       <c r="C429" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6171,7 +6171,7 @@
         <v>414</v>
       </c>
       <c r="C430" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6182,7 +6182,7 @@
         <v>415</v>
       </c>
       <c r="C431" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6193,7 +6193,7 @@
         <v>416</v>
       </c>
       <c r="C432" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6204,7 +6204,7 @@
         <v>417</v>
       </c>
       <c r="C433" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6215,7 +6215,7 @@
         <v>418</v>
       </c>
       <c r="C434" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6226,7 +6226,7 @@
         <v>419</v>
       </c>
       <c r="C435" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6237,7 +6237,7 @@
         <v>420</v>
       </c>
       <c r="C436" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6248,7 +6248,7 @@
         <v>421</v>
       </c>
       <c r="C437" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6259,7 +6259,7 @@
         <v>422</v>
       </c>
       <c r="C438" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6270,7 +6270,7 @@
         <v>423</v>
       </c>
       <c r="C439" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6281,7 +6281,7 @@
         <v>424</v>
       </c>
       <c r="C440" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6292,7 +6292,7 @@
         <v>425</v>
       </c>
       <c r="C441" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6303,7 +6303,7 @@
         <v>426</v>
       </c>
       <c r="C442" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6314,7 +6314,7 @@
         <v>427</v>
       </c>
       <c r="C443" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6325,7 +6325,7 @@
         <v>428</v>
       </c>
       <c r="C444" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6336,7 +6336,7 @@
         <v>429</v>
       </c>
       <c r="C445" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6347,7 +6347,7 @@
         <v>430</v>
       </c>
       <c r="C446" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6358,7 +6358,7 @@
         <v>431</v>
       </c>
       <c r="C447" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6369,7 +6369,7 @@
         <v>432</v>
       </c>
       <c r="C448" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6380,7 +6380,7 @@
         <v>433</v>
       </c>
       <c r="C449" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6391,7 +6391,7 @@
         <v>434</v>
       </c>
       <c r="C450" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6402,7 +6402,7 @@
         <v>435</v>
       </c>
       <c r="C451" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6413,7 +6413,7 @@
         <v>436</v>
       </c>
       <c r="C452" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6424,7 +6424,7 @@
         <v>437</v>
       </c>
       <c r="C453" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6435,7 +6435,7 @@
         <v>438</v>
       </c>
       <c r="C454" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6446,7 +6446,7 @@
         <v>439</v>
       </c>
       <c r="C455" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6457,7 +6457,7 @@
         <v>440</v>
       </c>
       <c r="C456" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6468,7 +6468,7 @@
         <v>441</v>
       </c>
       <c r="C457" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6479,7 +6479,7 @@
         <v>442</v>
       </c>
       <c r="C458" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6490,7 +6490,7 @@
         <v>443</v>
       </c>
       <c r="C459" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6501,7 +6501,7 @@
         <v>444</v>
       </c>
       <c r="C460" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6512,7 +6512,7 @@
         <v>445</v>
       </c>
       <c r="C461" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6523,7 +6523,7 @@
         <v>446</v>
       </c>
       <c r="C462" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6534,7 +6534,7 @@
         <v>447</v>
       </c>
       <c r="C463" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6545,7 +6545,7 @@
         <v>448</v>
       </c>
       <c r="C464" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6556,7 +6556,7 @@
         <v>449</v>
       </c>
       <c r="C465" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6567,7 +6567,7 @@
         <v>450</v>
       </c>
       <c r="C466" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6578,7 +6578,7 @@
         <v>451</v>
       </c>
       <c r="C467" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6589,7 +6589,7 @@
         <v>452</v>
       </c>
       <c r="C468" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6600,7 +6600,7 @@
         <v>453</v>
       </c>
       <c r="C469" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6620,7 +6620,7 @@
         <v>455</v>
       </c>
       <c r="C472" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6631,7 +6631,7 @@
         <v>456</v>
       </c>
       <c r="C473" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6642,7 +6642,7 @@
         <v>457</v>
       </c>
       <c r="C474" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6653,7 +6653,7 @@
         <v>458</v>
       </c>
       <c r="C475" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6664,7 +6664,7 @@
         <v>459</v>
       </c>
       <c r="C476" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6675,7 +6675,7 @@
         <v>460</v>
       </c>
       <c r="C477" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6686,7 +6686,7 @@
         <v>461</v>
       </c>
       <c r="C478" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6697,7 +6697,7 @@
         <v>462</v>
       </c>
       <c r="C479" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6708,7 +6708,7 @@
         <v>463</v>
       </c>
       <c r="C480" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6719,7 +6719,7 @@
         <v>464</v>
       </c>
       <c r="C481" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sort arrays of 0s 1s and 2s using dutch method.
</commit_message>
<xml_diff>
--- a/crashSheetDSA.xlsx
+++ b/crashSheetDSA.xlsx
@@ -52,10 +52,10 @@
     <t xml:space="preserve">Given an array which consists of only 0, 1 and 2. Sort the array without using any sorting algo</t>
   </si>
   <si>
+    <t xml:space="preserve">Move all the negative elements to one side of the array </t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;-&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move all the negative elements to one side of the array </t>
   </si>
   <si>
     <t xml:space="preserve">Find the Union and Intersection of the two sorted arrays.</t>
@@ -1658,11 +1658,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -1721,7 +1721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1737,10 +1737,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1751,7 +1751,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,7 +1762,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,7 +1773,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,7 +1784,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,7 +1795,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,7 +1806,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1817,7 +1817,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,7 +1828,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,7 +1839,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,7 +1850,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,7 +1861,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,7 +1872,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,7 +1883,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +1894,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,7 +1905,7 @@
         <v>26</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,7 +1916,7 @@
         <v>27</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,7 +1927,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,7 +1938,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,7 +1949,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1960,7 +1960,7 @@
         <v>31</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,7 +1971,7 @@
         <v>32</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,7 +1982,7 @@
         <v>33</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1993,7 +1993,7 @@
         <v>34</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,7 +2004,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,7 +2015,7 @@
         <v>36</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,7 +2026,7 @@
         <v>37</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2037,7 +2037,7 @@
         <v>38</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2048,7 +2048,7 @@
         <v>39</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,7 +2059,7 @@
         <v>40</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,7 +2070,7 @@
         <v>41</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2081,20 +2081,20 @@
         <v>42</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="7"/>
       <c r="C42" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
       <c r="C43" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,7 +2105,7 @@
         <v>44</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,7 +2116,7 @@
         <v>45</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2127,7 +2127,7 @@
         <v>46</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,7 +2138,7 @@
         <v>47</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,7 +2149,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,7 +2160,7 @@
         <v>49</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,7 +2171,7 @@
         <v>50</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2182,7 +2182,7 @@
         <v>51</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,7 +2193,7 @@
         <v>52</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,7 +2204,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,7 +2220,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,7 +2231,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,7 +2242,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,7 +2253,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,7 +2264,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2275,7 +2275,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,7 +2286,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,7 +2297,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,7 +2308,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,7 +2319,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,7 +2330,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,7 +2341,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2352,7 +2352,7 @@
         <v>67</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,7 +2363,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2374,7 +2374,7 @@
         <v>69</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,7 +2385,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,7 +2396,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,7 +2407,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,7 +2418,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2429,7 +2429,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2440,7 +2440,7 @@
         <v>75</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,7 +2451,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,7 +2462,7 @@
         <v>77</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,7 +2473,7 @@
         <v>78</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,7 +2484,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,7 +2495,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,7 +2506,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2517,7 +2517,7 @@
         <v>82</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,7 +2528,7 @@
         <v>83</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,7 +2539,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,7 +2550,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2561,7 +2561,7 @@
         <v>86</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,7 +2572,7 @@
         <v>87</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,7 +2583,7 @@
         <v>88</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,7 +2594,7 @@
         <v>89</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,7 +2605,7 @@
         <v>90</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2616,7 @@
         <v>91</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,7 +2627,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,7 +2638,7 @@
         <v>93</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2649,7 +2649,7 @@
         <v>94</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,7 +2660,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2671,7 +2671,7 @@
         <v>96</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,7 +2682,7 @@
         <v>97</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2698,7 +2698,7 @@
         <v>99</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,7 +2709,7 @@
         <v>100</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2720,7 +2720,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2731,7 +2731,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +2742,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,7 +2753,7 @@
         <v>104</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2764,7 +2764,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2775,7 +2775,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2786,7 +2786,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,7 +2797,7 @@
         <v>108</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2808,7 +2808,7 @@
         <v>109</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2819,7 +2819,7 @@
         <v>110</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,7 +2830,7 @@
         <v>111</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2841,7 +2841,7 @@
         <v>112</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2852,7 +2852,7 @@
         <v>113</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2863,7 +2863,7 @@
         <v>114</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2874,7 +2874,7 @@
         <v>115</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2885,7 +2885,7 @@
         <v>116</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2896,7 +2896,7 @@
         <v>117</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2907,7 +2907,7 @@
         <v>118</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2918,7 +2918,7 @@
         <v>119</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2929,7 +2929,7 @@
         <v>120</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2940,7 +2940,7 @@
         <v>121</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2951,7 +2951,7 @@
         <v>122</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,7 +2962,7 @@
         <v>123</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2973,7 +2973,7 @@
         <v>124</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2984,7 +2984,7 @@
         <v>125</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,7 +2995,7 @@
         <v>126</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3006,7 +3006,7 @@
         <v>127</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3017,7 +3017,7 @@
         <v>128</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,7 +3028,7 @@
         <v>129</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3039,7 +3039,7 @@
         <v>130</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3050,7 +3050,7 @@
         <v>131</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3061,7 +3061,7 @@
         <v>132</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3072,7 +3072,7 @@
         <v>133</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,7 +3083,7 @@
         <v>134</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3098,7 +3098,7 @@
         <v>136</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3109,7 +3109,7 @@
         <v>137</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3120,7 +3120,7 @@
         <v>138</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,7 +3131,7 @@
         <v>139</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3142,7 +3142,7 @@
         <v>140</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3153,7 +3153,7 @@
         <v>141</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,7 +3164,7 @@
         <v>142</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3175,7 +3175,7 @@
         <v>143</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,7 +3186,7 @@
         <v>144</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,7 +3197,7 @@
         <v>145</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3208,7 +3208,7 @@
         <v>146</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3219,7 +3219,7 @@
         <v>147</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3230,7 +3230,7 @@
         <v>148</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3241,7 +3241,7 @@
         <v>149</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,7 +3252,7 @@
         <v>150</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,7 +3263,7 @@
         <v>151</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,7 +3274,7 @@
         <v>152</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,7 +3285,7 @@
         <v>153</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,7 +3296,7 @@
         <v>154</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,7 +3307,7 @@
         <v>155</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3318,7 +3318,7 @@
         <v>156</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,7 +3329,7 @@
         <v>157</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3340,7 +3340,7 @@
         <v>158</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3351,7 +3351,7 @@
         <v>159</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3362,7 +3362,7 @@
         <v>160</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3373,7 +3373,7 @@
         <v>161</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3384,7 +3384,7 @@
         <v>162</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3395,7 +3395,7 @@
         <v>163</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3406,7 +3406,7 @@
         <v>164</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3417,7 +3417,7 @@
         <v>165</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3428,7 +3428,7 @@
         <v>166</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3439,7 +3439,7 @@
         <v>167</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3450,7 +3450,7 @@
         <v>168</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3461,7 +3461,7 @@
         <v>169</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,7 +3472,7 @@
         <v>170</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3483,7 +3483,7 @@
         <v>171</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3498,7 +3498,7 @@
         <v>173</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3509,7 +3509,7 @@
         <v>174</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3520,7 +3520,7 @@
         <v>175</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3531,7 +3531,7 @@
         <v>176</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3542,7 +3542,7 @@
         <v>177</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3553,7 +3553,7 @@
         <v>178</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3564,7 +3564,7 @@
         <v>179</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,7 +3575,7 @@
         <v>180</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3586,7 +3586,7 @@
         <v>181</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3597,7 +3597,7 @@
         <v>182</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3608,7 +3608,7 @@
         <v>183</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3619,7 +3619,7 @@
         <v>184</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3630,7 +3630,7 @@
         <v>185</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3641,7 +3641,7 @@
         <v>186</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3652,7 +3652,7 @@
         <v>187</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3663,7 +3663,7 @@
         <v>188</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3674,7 +3674,7 @@
         <v>189</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3685,7 +3685,7 @@
         <v>190</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3696,7 +3696,7 @@
         <v>191</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3707,7 +3707,7 @@
         <v>192</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3718,7 +3718,7 @@
         <v>193</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3729,7 +3729,7 @@
         <v>194</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3740,7 +3740,7 @@
         <v>195</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3751,7 +3751,7 @@
         <v>196</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3762,7 +3762,7 @@
         <v>197</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3773,7 +3773,7 @@
         <v>198</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,7 +3784,7 @@
         <v>199</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3795,7 +3795,7 @@
         <v>200</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3806,7 +3806,7 @@
         <v>201</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3817,7 +3817,7 @@
         <v>202</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3828,7 +3828,7 @@
         <v>203</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3839,7 +3839,7 @@
         <v>204</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3850,7 +3850,7 @@
         <v>205</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3861,7 +3861,7 @@
         <v>206</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3872,7 +3872,7 @@
         <v>207</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3893,7 +3893,7 @@
         <v>209</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3904,7 +3904,7 @@
         <v>210</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3915,7 +3915,7 @@
         <v>211</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3926,7 +3926,7 @@
         <v>212</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3937,7 +3937,7 @@
         <v>213</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3948,7 +3948,7 @@
         <v>214</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3959,7 +3959,7 @@
         <v>215</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3970,7 +3970,7 @@
         <v>216</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3981,7 +3981,7 @@
         <v>217</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3992,7 +3992,7 @@
         <v>218</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,7 +4003,7 @@
         <v>219</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4014,7 +4014,7 @@
         <v>220</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4025,7 +4025,7 @@
         <v>221</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4036,7 +4036,7 @@
         <v>222</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4047,7 +4047,7 @@
         <v>223</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4058,7 +4058,7 @@
         <v>224</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4069,7 +4069,7 @@
         <v>225</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4080,7 +4080,7 @@
         <v>226</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4091,7 +4091,7 @@
         <v>227</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4102,7 +4102,7 @@
         <v>228</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4113,7 +4113,7 @@
         <v>229</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4124,7 +4124,7 @@
         <v>230</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4143,7 +4143,7 @@
         <v>232</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4154,7 +4154,7 @@
         <v>233</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4165,7 +4165,7 @@
         <v>234</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4176,7 +4176,7 @@
         <v>235</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4187,7 +4187,7 @@
         <v>236</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4198,7 +4198,7 @@
         <v>237</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4209,7 +4209,7 @@
         <v>238</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4220,7 +4220,7 @@
         <v>239</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4231,7 +4231,7 @@
         <v>240</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4242,7 +4242,7 @@
         <v>241</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4253,7 +4253,7 @@
         <v>242</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4264,7 +4264,7 @@
         <v>243</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4275,7 +4275,7 @@
         <v>244</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4286,7 +4286,7 @@
         <v>245</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4297,7 +4297,7 @@
         <v>246</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4308,7 +4308,7 @@
         <v>247</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4319,7 +4319,7 @@
         <v>248</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4330,7 +4330,7 @@
         <v>249</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4341,7 +4341,7 @@
         <v>250</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4352,7 +4352,7 @@
         <v>251</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4363,7 +4363,7 @@
         <v>252</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,7 +4374,7 @@
         <v>253</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4385,7 +4385,7 @@
         <v>254</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4396,7 +4396,7 @@
         <v>255</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4407,7 +4407,7 @@
         <v>256</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4418,7 +4418,7 @@
         <v>257</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4429,7 +4429,7 @@
         <v>258</v>
       </c>
       <c r="C264" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4440,7 +4440,7 @@
         <v>259</v>
       </c>
       <c r="C265" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4451,7 +4451,7 @@
         <v>260</v>
       </c>
       <c r="C266" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4462,7 +4462,7 @@
         <v>261</v>
       </c>
       <c r="C267" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4473,7 +4473,7 @@
         <v>262</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4484,7 +4484,7 @@
         <v>263</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4495,7 +4495,7 @@
         <v>264</v>
       </c>
       <c r="C270" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4506,7 +4506,7 @@
         <v>88</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4517,7 +4517,7 @@
         <v>265</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,7 +4536,7 @@
         <v>267</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4547,7 +4547,7 @@
         <v>268</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4558,7 +4558,7 @@
         <v>269</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4569,7 +4569,7 @@
         <v>270</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4580,7 +4580,7 @@
         <v>271</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4591,7 +4591,7 @@
         <v>272</v>
       </c>
       <c r="C280" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4602,7 +4602,7 @@
         <v>273</v>
       </c>
       <c r="C281" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4613,7 +4613,7 @@
         <v>274</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4624,7 +4624,7 @@
         <v>275</v>
       </c>
       <c r="C283" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4635,7 +4635,7 @@
         <v>276</v>
       </c>
       <c r="C284" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4646,7 +4646,7 @@
         <v>277</v>
       </c>
       <c r="C285" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4657,7 +4657,7 @@
         <v>278</v>
       </c>
       <c r="C286" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4668,7 +4668,7 @@
         <v>279</v>
       </c>
       <c r="C287" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4679,7 +4679,7 @@
         <v>280</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4690,7 +4690,7 @@
         <v>281</v>
       </c>
       <c r="C289" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4701,7 +4701,7 @@
         <v>282</v>
       </c>
       <c r="C290" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4712,7 +4712,7 @@
         <v>283</v>
       </c>
       <c r="C291" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4723,7 +4723,7 @@
         <v>284</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4734,7 +4734,7 @@
         <v>285</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4753,7 +4753,7 @@
         <v>287</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4764,7 +4764,7 @@
         <v>288</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4775,7 +4775,7 @@
         <v>289</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4786,7 +4786,7 @@
         <v>290</v>
       </c>
       <c r="C299" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4797,7 +4797,7 @@
         <v>291</v>
       </c>
       <c r="C300" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4808,7 +4808,7 @@
         <v>292</v>
       </c>
       <c r="C301" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4819,7 +4819,7 @@
         <v>293</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4830,7 +4830,7 @@
         <v>294</v>
       </c>
       <c r="C303" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4841,7 +4841,7 @@
         <v>295</v>
       </c>
       <c r="C304" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4852,7 +4852,7 @@
         <v>296</v>
       </c>
       <c r="C305" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4863,7 +4863,7 @@
         <v>297</v>
       </c>
       <c r="C306" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4874,7 +4874,7 @@
         <v>298</v>
       </c>
       <c r="C307" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4885,7 +4885,7 @@
         <v>299</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4896,7 +4896,7 @@
         <v>300</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4907,7 +4907,7 @@
         <v>301</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4918,7 +4918,7 @@
         <v>302</v>
       </c>
       <c r="C311" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4929,7 +4929,7 @@
         <v>303</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4940,7 +4940,7 @@
         <v>304</v>
       </c>
       <c r="C313" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4951,7 +4951,7 @@
         <v>305</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4962,7 +4962,7 @@
         <v>306</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4973,7 +4973,7 @@
         <v>307</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4984,7 +4984,7 @@
         <v>308</v>
       </c>
       <c r="C317" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4995,7 +4995,7 @@
         <v>309</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5006,7 +5006,7 @@
         <v>310</v>
       </c>
       <c r="C319" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5017,7 +5017,7 @@
         <v>311</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5028,7 +5028,7 @@
         <v>312</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5039,7 +5039,7 @@
         <v>313</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5050,7 +5050,7 @@
         <v>314</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5061,7 +5061,7 @@
         <v>315</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5072,7 +5072,7 @@
         <v>316</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5083,7 +5083,7 @@
         <v>317</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5094,7 +5094,7 @@
         <v>318</v>
       </c>
       <c r="C327" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5105,7 +5105,7 @@
         <v>319</v>
       </c>
       <c r="C328" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5116,7 +5116,7 @@
         <v>320</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5127,7 +5127,7 @@
         <v>321</v>
       </c>
       <c r="C330" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5138,7 +5138,7 @@
         <v>322</v>
       </c>
       <c r="C331" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5149,7 +5149,7 @@
         <v>323</v>
       </c>
       <c r="C332" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5160,7 +5160,7 @@
         <v>324</v>
       </c>
       <c r="C333" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5179,7 +5179,7 @@
         <v>326</v>
       </c>
       <c r="C336" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5190,7 +5190,7 @@
         <v>327</v>
       </c>
       <c r="C337" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5201,7 +5201,7 @@
         <v>328</v>
       </c>
       <c r="C338" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5212,7 +5212,7 @@
         <v>329</v>
       </c>
       <c r="C339" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5223,7 +5223,7 @@
         <v>330</v>
       </c>
       <c r="C340" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5234,7 +5234,7 @@
         <v>331</v>
       </c>
       <c r="C341" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5245,7 +5245,7 @@
         <v>332</v>
       </c>
       <c r="C342" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5256,7 +5256,7 @@
         <v>333</v>
       </c>
       <c r="C343" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,7 +5267,7 @@
         <v>334</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5278,7 +5278,7 @@
         <v>335</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5289,7 +5289,7 @@
         <v>336</v>
       </c>
       <c r="C346" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5300,7 +5300,7 @@
         <v>337</v>
       </c>
       <c r="C347" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5311,7 +5311,7 @@
         <v>338</v>
       </c>
       <c r="C348" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5322,7 +5322,7 @@
         <v>339</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5333,7 +5333,7 @@
         <v>340</v>
       </c>
       <c r="C350" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5344,7 +5344,7 @@
         <v>341</v>
       </c>
       <c r="C351" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5355,7 +5355,7 @@
         <v>342</v>
       </c>
       <c r="C352" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5366,7 +5366,7 @@
         <v>343</v>
       </c>
       <c r="C353" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5385,7 +5385,7 @@
         <v>345</v>
       </c>
       <c r="C356" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5396,7 +5396,7 @@
         <v>346</v>
       </c>
       <c r="C357" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5407,7 +5407,7 @@
         <v>347</v>
       </c>
       <c r="C358" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5418,7 +5418,7 @@
         <v>348</v>
       </c>
       <c r="C359" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5429,7 +5429,7 @@
         <v>349</v>
       </c>
       <c r="C360" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5440,7 +5440,7 @@
         <v>350</v>
       </c>
       <c r="C361" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5451,7 +5451,7 @@
         <v>351</v>
       </c>
       <c r="C362" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5462,7 +5462,7 @@
         <v>352</v>
       </c>
       <c r="C363" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5473,7 +5473,7 @@
         <v>353</v>
       </c>
       <c r="C364" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5484,7 +5484,7 @@
         <v>354</v>
       </c>
       <c r="C365" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5495,7 +5495,7 @@
         <v>355</v>
       </c>
       <c r="C366" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5506,7 +5506,7 @@
         <v>356</v>
       </c>
       <c r="C367" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5517,7 +5517,7 @@
         <v>357</v>
       </c>
       <c r="C368" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5528,7 +5528,7 @@
         <v>358</v>
       </c>
       <c r="C369" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5539,7 +5539,7 @@
         <v>359</v>
       </c>
       <c r="C370" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5550,7 +5550,7 @@
         <v>360</v>
       </c>
       <c r="C371" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5561,7 +5561,7 @@
         <v>361</v>
       </c>
       <c r="C372" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5572,7 +5572,7 @@
         <v>362</v>
       </c>
       <c r="C373" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5583,7 +5583,7 @@
         <v>363</v>
       </c>
       <c r="C374" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5594,7 +5594,7 @@
         <v>364</v>
       </c>
       <c r="C375" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5605,7 +5605,7 @@
         <v>365</v>
       </c>
       <c r="C376" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5616,7 +5616,7 @@
         <v>366</v>
       </c>
       <c r="C377" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5627,7 +5627,7 @@
         <v>367</v>
       </c>
       <c r="C378" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5638,7 +5638,7 @@
         <v>368</v>
       </c>
       <c r="C379" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5649,7 +5649,7 @@
         <v>369</v>
       </c>
       <c r="C380" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5660,7 +5660,7 @@
         <v>370</v>
       </c>
       <c r="C381" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5671,7 +5671,7 @@
         <v>371</v>
       </c>
       <c r="C382" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5682,7 +5682,7 @@
         <v>372</v>
       </c>
       <c r="C383" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5693,7 +5693,7 @@
         <v>373</v>
       </c>
       <c r="C384" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5704,7 +5704,7 @@
         <v>374</v>
       </c>
       <c r="C385" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5715,7 +5715,7 @@
         <v>375</v>
       </c>
       <c r="C386" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5726,7 +5726,7 @@
         <v>376</v>
       </c>
       <c r="C387" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5737,7 +5737,7 @@
         <v>377</v>
       </c>
       <c r="C388" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5748,7 +5748,7 @@
         <v>378</v>
       </c>
       <c r="C389" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5759,7 +5759,7 @@
         <v>378</v>
       </c>
       <c r="C390" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5770,7 +5770,7 @@
         <v>379</v>
       </c>
       <c r="C391" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5781,7 +5781,7 @@
         <v>380</v>
       </c>
       <c r="C392" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5792,7 +5792,7 @@
         <v>381</v>
       </c>
       <c r="C393" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5803,7 +5803,7 @@
         <v>382</v>
       </c>
       <c r="C394" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,7 +5814,7 @@
         <v>383</v>
       </c>
       <c r="C395" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5825,7 +5825,7 @@
         <v>384</v>
       </c>
       <c r="C396" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5836,7 +5836,7 @@
         <v>385</v>
       </c>
       <c r="C397" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5847,7 +5847,7 @@
         <v>386</v>
       </c>
       <c r="C398" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5858,7 +5858,7 @@
         <v>387</v>
       </c>
       <c r="C399" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5877,7 +5877,7 @@
         <v>389</v>
       </c>
       <c r="C402" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5888,7 +5888,7 @@
         <v>390</v>
       </c>
       <c r="C403" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5899,7 +5899,7 @@
         <v>391</v>
       </c>
       <c r="C404" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5910,7 +5910,7 @@
         <v>90</v>
       </c>
       <c r="C405" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5921,7 +5921,7 @@
         <v>392</v>
       </c>
       <c r="C406" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5932,7 +5932,7 @@
         <v>393</v>
       </c>
       <c r="C407" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5951,7 +5951,7 @@
         <v>395</v>
       </c>
       <c r="C410" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5962,7 +5962,7 @@
         <v>396</v>
       </c>
       <c r="C411" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5973,7 +5973,7 @@
         <v>397</v>
       </c>
       <c r="C412" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5984,7 +5984,7 @@
         <v>398</v>
       </c>
       <c r="C413" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5995,7 +5995,7 @@
         <v>399</v>
       </c>
       <c r="C414" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6006,7 +6006,7 @@
         <v>400</v>
       </c>
       <c r="C415" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6017,7 +6017,7 @@
         <v>401</v>
       </c>
       <c r="C416" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6028,7 +6028,7 @@
         <v>274</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6039,7 +6039,7 @@
         <v>402</v>
       </c>
       <c r="C418" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6050,7 +6050,7 @@
         <v>403</v>
       </c>
       <c r="C419" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6061,7 +6061,7 @@
         <v>404</v>
       </c>
       <c r="C420" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6072,7 +6072,7 @@
         <v>405</v>
       </c>
       <c r="C421" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6083,7 +6083,7 @@
         <v>406</v>
       </c>
       <c r="C422" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6094,7 +6094,7 @@
         <v>407</v>
       </c>
       <c r="C423" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6105,7 +6105,7 @@
         <v>408</v>
       </c>
       <c r="C424" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6116,7 +6116,7 @@
         <v>409</v>
       </c>
       <c r="C425" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6127,7 +6127,7 @@
         <v>410</v>
       </c>
       <c r="C426" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6138,7 +6138,7 @@
         <v>411</v>
       </c>
       <c r="C427" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6149,7 +6149,7 @@
         <v>412</v>
       </c>
       <c r="C428" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6160,7 +6160,7 @@
         <v>413</v>
       </c>
       <c r="C429" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6171,7 +6171,7 @@
         <v>414</v>
       </c>
       <c r="C430" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6182,7 +6182,7 @@
         <v>415</v>
       </c>
       <c r="C431" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6193,7 +6193,7 @@
         <v>416</v>
       </c>
       <c r="C432" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6204,7 +6204,7 @@
         <v>417</v>
       </c>
       <c r="C433" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6215,7 +6215,7 @@
         <v>418</v>
       </c>
       <c r="C434" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6226,7 +6226,7 @@
         <v>419</v>
       </c>
       <c r="C435" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6237,7 +6237,7 @@
         <v>420</v>
       </c>
       <c r="C436" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6248,7 +6248,7 @@
         <v>421</v>
       </c>
       <c r="C437" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6259,7 +6259,7 @@
         <v>422</v>
       </c>
       <c r="C438" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6270,7 +6270,7 @@
         <v>423</v>
       </c>
       <c r="C439" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6281,7 +6281,7 @@
         <v>424</v>
       </c>
       <c r="C440" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6292,7 +6292,7 @@
         <v>425</v>
       </c>
       <c r="C441" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6303,7 +6303,7 @@
         <v>426</v>
       </c>
       <c r="C442" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6314,7 +6314,7 @@
         <v>427</v>
       </c>
       <c r="C443" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6325,7 +6325,7 @@
         <v>428</v>
       </c>
       <c r="C444" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6336,7 +6336,7 @@
         <v>429</v>
       </c>
       <c r="C445" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6347,7 +6347,7 @@
         <v>430</v>
       </c>
       <c r="C446" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6358,7 +6358,7 @@
         <v>431</v>
       </c>
       <c r="C447" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6369,7 +6369,7 @@
         <v>432</v>
       </c>
       <c r="C448" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6380,7 +6380,7 @@
         <v>433</v>
       </c>
       <c r="C449" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6391,7 +6391,7 @@
         <v>434</v>
       </c>
       <c r="C450" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6402,7 +6402,7 @@
         <v>435</v>
       </c>
       <c r="C451" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6413,7 +6413,7 @@
         <v>436</v>
       </c>
       <c r="C452" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6424,7 +6424,7 @@
         <v>437</v>
       </c>
       <c r="C453" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6435,7 +6435,7 @@
         <v>438</v>
       </c>
       <c r="C454" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6446,7 +6446,7 @@
         <v>439</v>
       </c>
       <c r="C455" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6457,7 +6457,7 @@
         <v>440</v>
       </c>
       <c r="C456" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6468,7 +6468,7 @@
         <v>441</v>
       </c>
       <c r="C457" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6479,7 +6479,7 @@
         <v>442</v>
       </c>
       <c r="C458" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6490,7 +6490,7 @@
         <v>443</v>
       </c>
       <c r="C459" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6501,7 +6501,7 @@
         <v>444</v>
       </c>
       <c r="C460" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6512,7 +6512,7 @@
         <v>445</v>
       </c>
       <c r="C461" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6523,7 +6523,7 @@
         <v>446</v>
       </c>
       <c r="C462" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6534,7 +6534,7 @@
         <v>447</v>
       </c>
       <c r="C463" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6545,7 +6545,7 @@
         <v>448</v>
       </c>
       <c r="C464" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6556,7 +6556,7 @@
         <v>449</v>
       </c>
       <c r="C465" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6567,7 +6567,7 @@
         <v>450</v>
       </c>
       <c r="C466" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6578,7 +6578,7 @@
         <v>451</v>
       </c>
       <c r="C467" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6589,7 +6589,7 @@
         <v>452</v>
       </c>
       <c r="C468" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6600,7 +6600,7 @@
         <v>453</v>
       </c>
       <c r="C469" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6620,7 +6620,7 @@
         <v>455</v>
       </c>
       <c r="C472" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6631,7 +6631,7 @@
         <v>456</v>
       </c>
       <c r="C473" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6642,7 +6642,7 @@
         <v>457</v>
       </c>
       <c r="C474" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6653,7 +6653,7 @@
         <v>458</v>
       </c>
       <c r="C475" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6664,7 +6664,7 @@
         <v>459</v>
       </c>
       <c r="C476" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6675,7 +6675,7 @@
         <v>460</v>
       </c>
       <c r="C477" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6686,7 +6686,7 @@
         <v>461</v>
       </c>
       <c r="C478" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6697,7 +6697,7 @@
         <v>462</v>
       </c>
       <c r="C479" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6708,7 +6708,7 @@
         <v>463</v>
       </c>
       <c r="C480" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6719,7 +6719,7 @@
         <v>464</v>
       </c>
       <c r="C481" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regular update- arrays and string
</commit_message>
<xml_diff>
--- a/crashSheetDSA.xlsx
+++ b/crashSheetDSA.xlsx
@@ -55,10 +55,10 @@
     <t xml:space="preserve">Move all the negative elements to one side of the array </t>
   </si>
   <si>
+    <t xml:space="preserve">Find the Union and Intersection of the two sorted arrays.</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;-&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Find the Union and Intersection of the two sorted arrays.</t>
   </si>
   <si>
     <t xml:space="preserve">Write a program to cyclically rotate an array by one.</t>
@@ -1658,11 +1658,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -1740,7 +1740,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,10 +1748,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,7 +1762,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,7 +1773,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,7 +1784,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,7 +1795,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,7 +1806,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1817,7 +1817,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,7 +1828,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,7 +1839,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,7 +1850,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,7 +1861,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,7 +1872,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,7 +1883,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +1894,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,7 +1905,7 @@
         <v>26</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,7 +1916,7 @@
         <v>27</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,7 +1927,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,7 +1938,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,7 +1949,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1960,7 +1960,7 @@
         <v>31</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,7 +1971,7 @@
         <v>32</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,7 +1982,7 @@
         <v>33</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1993,7 +1993,7 @@
         <v>34</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,7 +2004,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,7 +2015,7 @@
         <v>36</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,7 +2026,7 @@
         <v>37</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2037,7 +2037,7 @@
         <v>38</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2048,7 +2048,7 @@
         <v>39</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,7 +2059,7 @@
         <v>40</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,7 +2070,7 @@
         <v>41</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2081,20 +2081,20 @@
         <v>42</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="7"/>
       <c r="C42" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
       <c r="C43" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,7 +2105,7 @@
         <v>44</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,7 +2116,7 @@
         <v>45</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2127,7 +2127,7 @@
         <v>46</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,7 +2138,7 @@
         <v>47</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,7 +2149,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,7 +2160,7 @@
         <v>49</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,7 +2171,7 @@
         <v>50</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2182,7 +2182,7 @@
         <v>51</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,7 +2193,7 @@
         <v>52</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,7 +2204,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,7 +2220,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,7 +2231,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,7 +2242,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,7 +2253,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,7 +2264,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2275,7 +2275,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,7 +2286,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,7 +2297,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,7 +2308,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,7 +2319,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,7 +2330,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,7 +2341,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2352,7 +2352,7 @@
         <v>67</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,7 +2363,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2374,7 +2374,7 @@
         <v>69</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,7 +2385,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,7 +2396,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,7 +2407,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,7 +2418,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2429,7 +2429,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2440,7 +2440,7 @@
         <v>75</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,7 +2451,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,7 +2462,7 @@
         <v>77</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,7 +2473,7 @@
         <v>78</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,7 +2484,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,7 +2495,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,7 +2506,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2517,7 +2517,7 @@
         <v>82</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,7 +2528,7 @@
         <v>83</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,7 +2539,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,7 +2550,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2561,7 +2561,7 @@
         <v>86</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,7 +2572,7 @@
         <v>87</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,7 +2583,7 @@
         <v>88</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,7 +2594,7 @@
         <v>89</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,7 +2605,7 @@
         <v>90</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2616,7 @@
         <v>91</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,7 +2627,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,7 +2638,7 @@
         <v>93</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2649,7 +2649,7 @@
         <v>94</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,7 +2660,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2671,7 +2671,7 @@
         <v>96</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,7 +2682,7 @@
         <v>97</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2698,7 +2698,7 @@
         <v>99</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,7 +2709,7 @@
         <v>100</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2720,7 +2720,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2731,7 +2731,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +2742,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,7 +2753,7 @@
         <v>104</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2764,7 +2764,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2775,7 +2775,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2786,7 +2786,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,7 +2797,7 @@
         <v>108</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2808,7 +2808,7 @@
         <v>109</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2819,7 +2819,7 @@
         <v>110</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,7 +2830,7 @@
         <v>111</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2841,7 +2841,7 @@
         <v>112</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2852,7 +2852,7 @@
         <v>113</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2863,7 +2863,7 @@
         <v>114</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2874,7 +2874,7 @@
         <v>115</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2885,7 +2885,7 @@
         <v>116</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2896,7 +2896,7 @@
         <v>117</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2907,7 +2907,7 @@
         <v>118</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2918,7 +2918,7 @@
         <v>119</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2929,7 +2929,7 @@
         <v>120</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2940,7 +2940,7 @@
         <v>121</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2951,7 +2951,7 @@
         <v>122</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,7 +2962,7 @@
         <v>123</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2973,7 +2973,7 @@
         <v>124</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2984,7 +2984,7 @@
         <v>125</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,7 +2995,7 @@
         <v>126</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3006,7 +3006,7 @@
         <v>127</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3017,7 +3017,7 @@
         <v>128</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,7 +3028,7 @@
         <v>129</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3039,7 +3039,7 @@
         <v>130</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3050,7 +3050,7 @@
         <v>131</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3061,7 +3061,7 @@
         <v>132</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3072,7 +3072,7 @@
         <v>133</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,7 +3083,7 @@
         <v>134</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3098,7 +3098,7 @@
         <v>136</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3109,7 +3109,7 @@
         <v>137</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3120,7 +3120,7 @@
         <v>138</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,7 +3131,7 @@
         <v>139</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3142,7 +3142,7 @@
         <v>140</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3153,7 +3153,7 @@
         <v>141</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,7 +3164,7 @@
         <v>142</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3175,7 +3175,7 @@
         <v>143</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,7 +3186,7 @@
         <v>144</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,7 +3197,7 @@
         <v>145</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3208,7 +3208,7 @@
         <v>146</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3219,7 +3219,7 @@
         <v>147</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3230,7 +3230,7 @@
         <v>148</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3241,7 +3241,7 @@
         <v>149</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,7 +3252,7 @@
         <v>150</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,7 +3263,7 @@
         <v>151</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,7 +3274,7 @@
         <v>152</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,7 +3285,7 @@
         <v>153</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,7 +3296,7 @@
         <v>154</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,7 +3307,7 @@
         <v>155</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3318,7 +3318,7 @@
         <v>156</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,7 +3329,7 @@
         <v>157</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3340,7 +3340,7 @@
         <v>158</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3351,7 +3351,7 @@
         <v>159</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3362,7 +3362,7 @@
         <v>160</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3373,7 +3373,7 @@
         <v>161</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3384,7 +3384,7 @@
         <v>162</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3395,7 +3395,7 @@
         <v>163</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3406,7 +3406,7 @@
         <v>164</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3417,7 +3417,7 @@
         <v>165</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3428,7 +3428,7 @@
         <v>166</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3439,7 +3439,7 @@
         <v>167</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3450,7 +3450,7 @@
         <v>168</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3461,7 +3461,7 @@
         <v>169</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,7 +3472,7 @@
         <v>170</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3483,7 +3483,7 @@
         <v>171</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3498,7 +3498,7 @@
         <v>173</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3509,7 +3509,7 @@
         <v>174</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3520,7 +3520,7 @@
         <v>175</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3531,7 +3531,7 @@
         <v>176</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3542,7 +3542,7 @@
         <v>177</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3553,7 +3553,7 @@
         <v>178</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3564,7 +3564,7 @@
         <v>179</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,7 +3575,7 @@
         <v>180</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3586,7 +3586,7 @@
         <v>181</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3597,7 +3597,7 @@
         <v>182</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3608,7 +3608,7 @@
         <v>183</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3619,7 +3619,7 @@
         <v>184</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3630,7 +3630,7 @@
         <v>185</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3641,7 +3641,7 @@
         <v>186</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3652,7 +3652,7 @@
         <v>187</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3663,7 +3663,7 @@
         <v>188</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3674,7 +3674,7 @@
         <v>189</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3685,7 +3685,7 @@
         <v>190</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3696,7 +3696,7 @@
         <v>191</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3707,7 +3707,7 @@
         <v>192</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3718,7 +3718,7 @@
         <v>193</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3729,7 +3729,7 @@
         <v>194</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3740,7 +3740,7 @@
         <v>195</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3751,7 +3751,7 @@
         <v>196</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3762,7 +3762,7 @@
         <v>197</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3773,7 +3773,7 @@
         <v>198</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,7 +3784,7 @@
         <v>199</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3795,7 +3795,7 @@
         <v>200</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3806,7 +3806,7 @@
         <v>201</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3817,7 +3817,7 @@
         <v>202</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3828,7 +3828,7 @@
         <v>203</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3839,7 +3839,7 @@
         <v>204</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3850,7 +3850,7 @@
         <v>205</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3861,7 +3861,7 @@
         <v>206</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3872,7 +3872,7 @@
         <v>207</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3893,7 +3893,7 @@
         <v>209</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3904,7 +3904,7 @@
         <v>210</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3915,7 +3915,7 @@
         <v>211</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3926,7 +3926,7 @@
         <v>212</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3937,7 +3937,7 @@
         <v>213</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3948,7 +3948,7 @@
         <v>214</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3959,7 +3959,7 @@
         <v>215</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3970,7 +3970,7 @@
         <v>216</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3981,7 +3981,7 @@
         <v>217</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3992,7 +3992,7 @@
         <v>218</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,7 +4003,7 @@
         <v>219</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4014,7 +4014,7 @@
         <v>220</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4025,7 +4025,7 @@
         <v>221</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4036,7 +4036,7 @@
         <v>222</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4047,7 +4047,7 @@
         <v>223</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4058,7 +4058,7 @@
         <v>224</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4069,7 +4069,7 @@
         <v>225</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4080,7 +4080,7 @@
         <v>226</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4091,7 +4091,7 @@
         <v>227</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4102,7 +4102,7 @@
         <v>228</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4113,7 +4113,7 @@
         <v>229</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4124,7 +4124,7 @@
         <v>230</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4143,7 +4143,7 @@
         <v>232</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4154,7 +4154,7 @@
         <v>233</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4165,7 +4165,7 @@
         <v>234</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4176,7 +4176,7 @@
         <v>235</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4187,7 +4187,7 @@
         <v>236</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4198,7 +4198,7 @@
         <v>237</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4209,7 +4209,7 @@
         <v>238</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4220,7 +4220,7 @@
         <v>239</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4231,7 +4231,7 @@
         <v>240</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4242,7 +4242,7 @@
         <v>241</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4253,7 +4253,7 @@
         <v>242</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4264,7 +4264,7 @@
         <v>243</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4275,7 +4275,7 @@
         <v>244</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4286,7 +4286,7 @@
         <v>245</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4297,7 +4297,7 @@
         <v>246</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4308,7 +4308,7 @@
         <v>247</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4319,7 +4319,7 @@
         <v>248</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4330,7 +4330,7 @@
         <v>249</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4341,7 +4341,7 @@
         <v>250</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4352,7 +4352,7 @@
         <v>251</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4363,7 +4363,7 @@
         <v>252</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,7 +4374,7 @@
         <v>253</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4385,7 +4385,7 @@
         <v>254</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4396,7 +4396,7 @@
         <v>255</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4407,7 +4407,7 @@
         <v>256</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4418,7 +4418,7 @@
         <v>257</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4429,7 +4429,7 @@
         <v>258</v>
       </c>
       <c r="C264" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4440,7 +4440,7 @@
         <v>259</v>
       </c>
       <c r="C265" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4451,7 +4451,7 @@
         <v>260</v>
       </c>
       <c r="C266" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4462,7 +4462,7 @@
         <v>261</v>
       </c>
       <c r="C267" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4473,7 +4473,7 @@
         <v>262</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4484,7 +4484,7 @@
         <v>263</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4495,7 +4495,7 @@
         <v>264</v>
       </c>
       <c r="C270" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4506,7 +4506,7 @@
         <v>88</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4517,7 +4517,7 @@
         <v>265</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,7 +4536,7 @@
         <v>267</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4547,7 +4547,7 @@
         <v>268</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4558,7 +4558,7 @@
         <v>269</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4569,7 +4569,7 @@
         <v>270</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4580,7 +4580,7 @@
         <v>271</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4591,7 +4591,7 @@
         <v>272</v>
       </c>
       <c r="C280" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4602,7 +4602,7 @@
         <v>273</v>
       </c>
       <c r="C281" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4613,7 +4613,7 @@
         <v>274</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4624,7 +4624,7 @@
         <v>275</v>
       </c>
       <c r="C283" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4635,7 +4635,7 @@
         <v>276</v>
       </c>
       <c r="C284" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4646,7 +4646,7 @@
         <v>277</v>
       </c>
       <c r="C285" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4657,7 +4657,7 @@
         <v>278</v>
       </c>
       <c r="C286" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4668,7 +4668,7 @@
         <v>279</v>
       </c>
       <c r="C287" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4679,7 +4679,7 @@
         <v>280</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4690,7 +4690,7 @@
         <v>281</v>
       </c>
       <c r="C289" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4701,7 +4701,7 @@
         <v>282</v>
       </c>
       <c r="C290" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4712,7 +4712,7 @@
         <v>283</v>
       </c>
       <c r="C291" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4723,7 +4723,7 @@
         <v>284</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4734,7 +4734,7 @@
         <v>285</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4753,7 +4753,7 @@
         <v>287</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4764,7 +4764,7 @@
         <v>288</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4775,7 +4775,7 @@
         <v>289</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4786,7 +4786,7 @@
         <v>290</v>
       </c>
       <c r="C299" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4797,7 +4797,7 @@
         <v>291</v>
       </c>
       <c r="C300" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4808,7 +4808,7 @@
         <v>292</v>
       </c>
       <c r="C301" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4819,7 +4819,7 @@
         <v>293</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4830,7 +4830,7 @@
         <v>294</v>
       </c>
       <c r="C303" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4841,7 +4841,7 @@
         <v>295</v>
       </c>
       <c r="C304" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4852,7 +4852,7 @@
         <v>296</v>
       </c>
       <c r="C305" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4863,7 +4863,7 @@
         <v>297</v>
       </c>
       <c r="C306" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4874,7 +4874,7 @@
         <v>298</v>
       </c>
       <c r="C307" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4885,7 +4885,7 @@
         <v>299</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4896,7 +4896,7 @@
         <v>300</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4907,7 +4907,7 @@
         <v>301</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4918,7 +4918,7 @@
         <v>302</v>
       </c>
       <c r="C311" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4929,7 +4929,7 @@
         <v>303</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4940,7 +4940,7 @@
         <v>304</v>
       </c>
       <c r="C313" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4951,7 +4951,7 @@
         <v>305</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4962,7 +4962,7 @@
         <v>306</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4973,7 +4973,7 @@
         <v>307</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4984,7 +4984,7 @@
         <v>308</v>
       </c>
       <c r="C317" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4995,7 +4995,7 @@
         <v>309</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5006,7 +5006,7 @@
         <v>310</v>
       </c>
       <c r="C319" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5017,7 +5017,7 @@
         <v>311</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5028,7 +5028,7 @@
         <v>312</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5039,7 +5039,7 @@
         <v>313</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5050,7 +5050,7 @@
         <v>314</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5061,7 +5061,7 @@
         <v>315</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5072,7 +5072,7 @@
         <v>316</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5083,7 +5083,7 @@
         <v>317</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5094,7 +5094,7 @@
         <v>318</v>
       </c>
       <c r="C327" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5105,7 +5105,7 @@
         <v>319</v>
       </c>
       <c r="C328" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5116,7 +5116,7 @@
         <v>320</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5127,7 +5127,7 @@
         <v>321</v>
       </c>
       <c r="C330" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5138,7 +5138,7 @@
         <v>322</v>
       </c>
       <c r="C331" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5149,7 +5149,7 @@
         <v>323</v>
       </c>
       <c r="C332" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5160,7 +5160,7 @@
         <v>324</v>
       </c>
       <c r="C333" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5179,7 +5179,7 @@
         <v>326</v>
       </c>
       <c r="C336" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5190,7 +5190,7 @@
         <v>327</v>
       </c>
       <c r="C337" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5201,7 +5201,7 @@
         <v>328</v>
       </c>
       <c r="C338" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5212,7 +5212,7 @@
         <v>329</v>
       </c>
       <c r="C339" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5223,7 +5223,7 @@
         <v>330</v>
       </c>
       <c r="C340" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5234,7 +5234,7 @@
         <v>331</v>
       </c>
       <c r="C341" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5245,7 +5245,7 @@
         <v>332</v>
       </c>
       <c r="C342" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5256,7 +5256,7 @@
         <v>333</v>
       </c>
       <c r="C343" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,7 +5267,7 @@
         <v>334</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5278,7 +5278,7 @@
         <v>335</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5289,7 +5289,7 @@
         <v>336</v>
       </c>
       <c r="C346" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5300,7 +5300,7 @@
         <v>337</v>
       </c>
       <c r="C347" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5311,7 +5311,7 @@
         <v>338</v>
       </c>
       <c r="C348" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5322,7 +5322,7 @@
         <v>339</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5333,7 +5333,7 @@
         <v>340</v>
       </c>
       <c r="C350" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5344,7 +5344,7 @@
         <v>341</v>
       </c>
       <c r="C351" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5355,7 +5355,7 @@
         <v>342</v>
       </c>
       <c r="C352" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5366,7 +5366,7 @@
         <v>343</v>
       </c>
       <c r="C353" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5385,7 +5385,7 @@
         <v>345</v>
       </c>
       <c r="C356" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5396,7 +5396,7 @@
         <v>346</v>
       </c>
       <c r="C357" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5407,7 +5407,7 @@
         <v>347</v>
       </c>
       <c r="C358" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5418,7 +5418,7 @@
         <v>348</v>
       </c>
       <c r="C359" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5429,7 +5429,7 @@
         <v>349</v>
       </c>
       <c r="C360" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5440,7 +5440,7 @@
         <v>350</v>
       </c>
       <c r="C361" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5451,7 +5451,7 @@
         <v>351</v>
       </c>
       <c r="C362" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5462,7 +5462,7 @@
         <v>352</v>
       </c>
       <c r="C363" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5473,7 +5473,7 @@
         <v>353</v>
       </c>
       <c r="C364" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5484,7 +5484,7 @@
         <v>354</v>
       </c>
       <c r="C365" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5495,7 +5495,7 @@
         <v>355</v>
       </c>
       <c r="C366" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5506,7 +5506,7 @@
         <v>356</v>
       </c>
       <c r="C367" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5517,7 +5517,7 @@
         <v>357</v>
       </c>
       <c r="C368" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5528,7 +5528,7 @@
         <v>358</v>
       </c>
       <c r="C369" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5539,7 +5539,7 @@
         <v>359</v>
       </c>
       <c r="C370" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5550,7 +5550,7 @@
         <v>360</v>
       </c>
       <c r="C371" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5561,7 +5561,7 @@
         <v>361</v>
       </c>
       <c r="C372" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5572,7 +5572,7 @@
         <v>362</v>
       </c>
       <c r="C373" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5583,7 +5583,7 @@
         <v>363</v>
       </c>
       <c r="C374" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5594,7 +5594,7 @@
         <v>364</v>
       </c>
       <c r="C375" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5605,7 +5605,7 @@
         <v>365</v>
       </c>
       <c r="C376" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5616,7 +5616,7 @@
         <v>366</v>
       </c>
       <c r="C377" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5627,7 +5627,7 @@
         <v>367</v>
       </c>
       <c r="C378" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5638,7 +5638,7 @@
         <v>368</v>
       </c>
       <c r="C379" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5649,7 +5649,7 @@
         <v>369</v>
       </c>
       <c r="C380" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5660,7 +5660,7 @@
         <v>370</v>
       </c>
       <c r="C381" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5671,7 +5671,7 @@
         <v>371</v>
       </c>
       <c r="C382" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5682,7 +5682,7 @@
         <v>372</v>
       </c>
       <c r="C383" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5693,7 +5693,7 @@
         <v>373</v>
       </c>
       <c r="C384" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5704,7 +5704,7 @@
         <v>374</v>
       </c>
       <c r="C385" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5715,7 +5715,7 @@
         <v>375</v>
       </c>
       <c r="C386" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5726,7 +5726,7 @@
         <v>376</v>
       </c>
       <c r="C387" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5737,7 +5737,7 @@
         <v>377</v>
       </c>
       <c r="C388" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5748,7 +5748,7 @@
         <v>378</v>
       </c>
       <c r="C389" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5759,7 +5759,7 @@
         <v>378</v>
       </c>
       <c r="C390" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5770,7 +5770,7 @@
         <v>379</v>
       </c>
       <c r="C391" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5781,7 +5781,7 @@
         <v>380</v>
       </c>
       <c r="C392" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5792,7 +5792,7 @@
         <v>381</v>
       </c>
       <c r="C393" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5803,7 +5803,7 @@
         <v>382</v>
       </c>
       <c r="C394" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,7 +5814,7 @@
         <v>383</v>
       </c>
       <c r="C395" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5825,7 +5825,7 @@
         <v>384</v>
       </c>
       <c r="C396" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5836,7 +5836,7 @@
         <v>385</v>
       </c>
       <c r="C397" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5847,7 +5847,7 @@
         <v>386</v>
       </c>
       <c r="C398" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5858,7 +5858,7 @@
         <v>387</v>
       </c>
       <c r="C399" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5877,7 +5877,7 @@
         <v>389</v>
       </c>
       <c r="C402" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5888,7 +5888,7 @@
         <v>390</v>
       </c>
       <c r="C403" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5899,7 +5899,7 @@
         <v>391</v>
       </c>
       <c r="C404" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5910,7 +5910,7 @@
         <v>90</v>
       </c>
       <c r="C405" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5921,7 +5921,7 @@
         <v>392</v>
       </c>
       <c r="C406" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5932,7 +5932,7 @@
         <v>393</v>
       </c>
       <c r="C407" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5951,7 +5951,7 @@
         <v>395</v>
       </c>
       <c r="C410" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5962,7 +5962,7 @@
         <v>396</v>
       </c>
       <c r="C411" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5973,7 +5973,7 @@
         <v>397</v>
       </c>
       <c r="C412" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5984,7 +5984,7 @@
         <v>398</v>
       </c>
       <c r="C413" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5995,7 +5995,7 @@
         <v>399</v>
       </c>
       <c r="C414" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6006,7 +6006,7 @@
         <v>400</v>
       </c>
       <c r="C415" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6017,7 +6017,7 @@
         <v>401</v>
       </c>
       <c r="C416" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6028,7 +6028,7 @@
         <v>274</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6039,7 +6039,7 @@
         <v>402</v>
       </c>
       <c r="C418" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6050,7 +6050,7 @@
         <v>403</v>
       </c>
       <c r="C419" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6061,7 +6061,7 @@
         <v>404</v>
       </c>
       <c r="C420" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6072,7 +6072,7 @@
         <v>405</v>
       </c>
       <c r="C421" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6083,7 +6083,7 @@
         <v>406</v>
       </c>
       <c r="C422" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6094,7 +6094,7 @@
         <v>407</v>
       </c>
       <c r="C423" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6105,7 +6105,7 @@
         <v>408</v>
       </c>
       <c r="C424" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6116,7 +6116,7 @@
         <v>409</v>
       </c>
       <c r="C425" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6127,7 +6127,7 @@
         <v>410</v>
       </c>
       <c r="C426" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6138,7 +6138,7 @@
         <v>411</v>
       </c>
       <c r="C427" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6149,7 +6149,7 @@
         <v>412</v>
       </c>
       <c r="C428" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6160,7 +6160,7 @@
         <v>413</v>
       </c>
       <c r="C429" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6171,7 +6171,7 @@
         <v>414</v>
       </c>
       <c r="C430" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6182,7 +6182,7 @@
         <v>415</v>
       </c>
       <c r="C431" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6193,7 +6193,7 @@
         <v>416</v>
       </c>
       <c r="C432" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6204,7 +6204,7 @@
         <v>417</v>
       </c>
       <c r="C433" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6215,7 +6215,7 @@
         <v>418</v>
       </c>
       <c r="C434" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6226,7 +6226,7 @@
         <v>419</v>
       </c>
       <c r="C435" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6237,7 +6237,7 @@
         <v>420</v>
       </c>
       <c r="C436" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6248,7 +6248,7 @@
         <v>421</v>
       </c>
       <c r="C437" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6259,7 +6259,7 @@
         <v>422</v>
       </c>
       <c r="C438" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6270,7 +6270,7 @@
         <v>423</v>
       </c>
       <c r="C439" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6281,7 +6281,7 @@
         <v>424</v>
       </c>
       <c r="C440" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6292,7 +6292,7 @@
         <v>425</v>
       </c>
       <c r="C441" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6303,7 +6303,7 @@
         <v>426</v>
       </c>
       <c r="C442" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6314,7 +6314,7 @@
         <v>427</v>
       </c>
       <c r="C443" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6325,7 +6325,7 @@
         <v>428</v>
       </c>
       <c r="C444" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6336,7 +6336,7 @@
         <v>429</v>
       </c>
       <c r="C445" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6347,7 +6347,7 @@
         <v>430</v>
       </c>
       <c r="C446" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6358,7 +6358,7 @@
         <v>431</v>
       </c>
       <c r="C447" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6369,7 +6369,7 @@
         <v>432</v>
       </c>
       <c r="C448" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6380,7 +6380,7 @@
         <v>433</v>
       </c>
       <c r="C449" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6391,7 +6391,7 @@
         <v>434</v>
       </c>
       <c r="C450" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6402,7 +6402,7 @@
         <v>435</v>
       </c>
       <c r="C451" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6413,7 +6413,7 @@
         <v>436</v>
       </c>
       <c r="C452" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6424,7 +6424,7 @@
         <v>437</v>
       </c>
       <c r="C453" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6435,7 +6435,7 @@
         <v>438</v>
       </c>
       <c r="C454" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6446,7 +6446,7 @@
         <v>439</v>
       </c>
       <c r="C455" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6457,7 +6457,7 @@
         <v>440</v>
       </c>
       <c r="C456" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6468,7 +6468,7 @@
         <v>441</v>
       </c>
       <c r="C457" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6479,7 +6479,7 @@
         <v>442</v>
       </c>
       <c r="C458" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6490,7 +6490,7 @@
         <v>443</v>
       </c>
       <c r="C459" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6501,7 +6501,7 @@
         <v>444</v>
       </c>
       <c r="C460" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6512,7 +6512,7 @@
         <v>445</v>
       </c>
       <c r="C461" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6523,7 +6523,7 @@
         <v>446</v>
       </c>
       <c r="C462" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6534,7 +6534,7 @@
         <v>447</v>
       </c>
       <c r="C463" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6545,7 +6545,7 @@
         <v>448</v>
       </c>
       <c r="C464" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6556,7 +6556,7 @@
         <v>449</v>
       </c>
       <c r="C465" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6567,7 +6567,7 @@
         <v>450</v>
       </c>
       <c r="C466" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6578,7 +6578,7 @@
         <v>451</v>
       </c>
       <c r="C467" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6589,7 +6589,7 @@
         <v>452</v>
       </c>
       <c r="C468" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6600,7 +6600,7 @@
         <v>453</v>
       </c>
       <c r="C469" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6620,7 +6620,7 @@
         <v>455</v>
       </c>
       <c r="C472" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6631,7 +6631,7 @@
         <v>456</v>
       </c>
       <c r="C473" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6642,7 +6642,7 @@
         <v>457</v>
       </c>
       <c r="C474" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6653,7 +6653,7 @@
         <v>458</v>
       </c>
       <c r="C475" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6664,7 +6664,7 @@
         <v>459</v>
       </c>
       <c r="C476" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6675,7 +6675,7 @@
         <v>460</v>
       </c>
       <c r="C477" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6686,7 +6686,7 @@
         <v>461</v>
       </c>
       <c r="C478" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6697,7 +6697,7 @@
         <v>462</v>
       </c>
       <c r="C479" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6708,7 +6708,7 @@
         <v>463</v>
       </c>
       <c r="C480" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6719,7 +6719,7 @@
         <v>464</v>
       </c>
       <c r="C481" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>